<commit_message>
More Searches added - finish Searches - figure out alorithum
</commit_message>
<xml_diff>
--- a/Implementation Code/Search Book.xlsx
+++ b/Implementation Code/Search Book.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +501,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>